<commit_message>
Done implement import data
</commit_message>
<xml_diff>
--- a/assets/files/data/Competition Schedules.xlsx
+++ b/assets/files/data/Competition Schedules.xlsx
@@ -584,6 +584,9 @@
     <t>manchester-united.png</t>
   </si>
   <si>
+    <t>Man Utd</t>
+  </si>
+  <si>
     <t>Steve McClaren</t>
   </si>
   <si>
@@ -1580,9 +1583,6 @@
     <t>Franco Soldati</t>
   </si>
   <si>
-    <t>France Ligue1</t>
-  </si>
-  <si>
     <t>Stéphane Moulin</t>
   </si>
   <si>
@@ -3224,7 +3224,7 @@
     <t>FC Augsburg 0-0 VfL Wolfsburg</t>
   </si>
   <si>
-    <t>Bayern Mun 2-0 Hertha BSC</t>
+    <t>Bayern Munich 2-0 Hertha BSC</t>
   </si>
   <si>
     <t>Hannover 96 4-0 FC Ingolstadt 04</t>
@@ -3233,25 +3233,25 @@
     <t>SV Werder Bremen 1-3 Hamburger SV</t>
   </si>
   <si>
-    <t>TSG 1899 Hoffenheim 3-3 B M'gladbach</t>
-  </si>
-  <si>
-    <t>1. FSV Mainz 05 2-1 Eintracht Frankfurt</t>
+    <t>Hoffenheim 3-3 B M'gladbach</t>
+  </si>
+  <si>
+    <t>Mainz 05 2-1 Eintracht Frankfurt</t>
   </si>
   <si>
     <t>Friday 27th November 2015</t>
   </si>
   <si>
-    <t>SV Darmstadt 98 0-0 1. FC Köln</t>
-  </si>
-  <si>
-    <t>Hertha BSC 1-0 TSG 1899 Hoffenheim</t>
-  </si>
-  <si>
-    <t>FC Ingolstadt 04 3-1 SV Darmstadt 98</t>
-  </si>
-  <si>
-    <t>1. FC Köln 0-0 1. FSV Mainz 05</t>
+    <t>Darmstadt 98 0-0 1. FC Köln</t>
+  </si>
+  <si>
+    <t>Hertha BSC 1-0 Hoffenheim</t>
+  </si>
+  <si>
+    <t>FC Ingolstadt 04 3-1 Darmstadt 98</t>
+  </si>
+  <si>
+    <t>1. FC Köln 0-0 Mainz 05</t>
   </si>
   <si>
     <t>B M'gladbach 2-1 Hannover 96</t>
@@ -3266,7 +3266,7 @@
     <t>VfB Stuttgart 0-4 FC Augsburg</t>
   </si>
   <si>
-    <t>Schalke 1-3 Bayern Mun</t>
+    <t>Schalke 1-3 Bayern Munich</t>
   </si>
   <si>
     <t>Friday 20th November 2015</t>
@@ -3281,7 +3281,7 @@
     <t>FC Augsburg 1-2 SV Werder Bremen</t>
   </si>
   <si>
-    <t>1. FSV Mainz 05 2-0 VfL Wolfsburg</t>
+    <t>Mainz 05 2-0 VfL Wolfsburg</t>
   </si>
   <si>
     <t>Bayer Levkn 1-2 1. FC Köln</t>
@@ -3290,13 +3290,13 @@
     <t>B M'gladbach 0-0 FC Ingolstadt 04</t>
   </si>
   <si>
-    <t>Bayern Mun 4-0 VfB Stuttgart</t>
-  </si>
-  <si>
-    <t>TSG 1899 Hoffenheim 0-0 Eintracht Frankfurt</t>
-  </si>
-  <si>
-    <t>SV Darmstadt 98 1-1 Hamburger SV</t>
+    <t>Bayern Munich 4-0 VfB Stuttgart</t>
+  </si>
+  <si>
+    <t>Hoffenheim 0-0 Eintracht Frankfurt</t>
+  </si>
+  <si>
+    <t>Darmstadt 98 1-1 Hamburger SV</t>
   </si>
   <si>
     <t>Friday 6th November 2015</t>
@@ -3305,16 +3305,16 @@
     <t>Hannover 96 1-3 Hertha BSC</t>
   </si>
   <si>
-    <t>VfB Stuttgart 2-0 SV Darmstadt 98</t>
+    <t>VfB Stuttgart 2-0 Darmstadt 98</t>
   </si>
   <si>
     <t>Hamburger SV 1-2 Hannover 96</t>
   </si>
   <si>
-    <t>1. FC Köln 0-0 TSG 1899 Hoffenheim</t>
-  </si>
-  <si>
-    <t>FC Augsburg 3-3 1. FSV Mainz 05</t>
+    <t>1. FC Köln 0-0 Hoffenheim</t>
+  </si>
+  <si>
+    <t>FC Augsburg 3-3 Mainz 05</t>
   </si>
   <si>
     <t>Schalke 1-1 FC Ingolstadt 04</t>
@@ -3332,7 +3332,7 @@
     <t>Friday 30th October 2015</t>
   </si>
   <si>
-    <t>Eintracht Frankfurt 0-0 Bayern Mun</t>
+    <t>Eintracht Frankfurt 0-0 Bayern Munich</t>
   </si>
   <si>
     <t>Dortmund 5-1 FC Augsburg</t>
@@ -3341,19 +3341,19 @@
     <t>B M'gladbach 3-1 Schalke</t>
   </si>
   <si>
-    <t>1. FSV Mainz 05 1-3 SV Werder Bremen</t>
+    <t>Mainz 05 1-3 SV Werder Bremen</t>
   </si>
   <si>
     <t>Bayer Levkn 4-3 VfB Stuttgart</t>
   </si>
   <si>
-    <t>Bayern Mun 4-0 1. FC Köln</t>
+    <t>Bayern Munich 4-0 1. FC Köln</t>
   </si>
   <si>
     <t>Hannover 96 1-2 Eintracht Frankfurt</t>
   </si>
   <si>
-    <t>SV Darmstadt 98 0-1 VfL Wolfsburg</t>
+    <t>Darmstadt 98 0-1 VfL Wolfsburg</t>
   </si>
   <si>
     <t>FC Ingolstadt 04 0-1 Hertha BSC</t>
@@ -3362,7 +3362,7 @@
     <t>Friday 23rd October 2015</t>
   </si>
   <si>
-    <t>TSG 1899 Hoffenheim 0-1 Hamburger SV</t>
+    <t>Hoffenheim 0-1 Hamburger SV</t>
   </si>
   <si>
     <t>1. FC Köln 0-1 Hannover 96</t>
@@ -3371,7 +3371,7 @@
     <t>VfB Stuttgart 1-0 FC Ingolstadt 04</t>
   </si>
   <si>
-    <t>FC Augsburg 0-2 SV Darmstadt 98</t>
+    <t>FC Augsburg 0-2 Darmstadt 98</t>
   </si>
   <si>
     <t>Schalke 2-1 Hertha BSC</t>
@@ -3380,10 +3380,10 @@
     <t>Hamburger SV 0-0 Bayer Levkn</t>
   </si>
   <si>
-    <t>SV Werder Bremen 0-1 Bayern Mun</t>
-  </si>
-  <si>
-    <t>VfL Wolfsburg 4-2 TSG 1899 Hoffenheim</t>
+    <t>SV Werder Bremen 0-1 Bayern Munich</t>
+  </si>
+  <si>
+    <t>VfL Wolfsburg 4-2 Hoffenheim</t>
   </si>
   <si>
     <t>Eintracht Frankfurt 1-5 B M'gladbach</t>
@@ -3392,7 +3392,7 @@
     <t>Friday 16th October 2015</t>
   </si>
   <si>
-    <t>1. FSV Mainz 05 0-2 Dortmund</t>
+    <t>Mainz 05 0-2 Dortmund</t>
   </si>
   <si>
     <t>Schalke 0-3 1. FC Köln</t>
@@ -3401,7 +3401,7 @@
     <t>Bayer Levkn 1-1 FC Augsburg</t>
   </si>
   <si>
-    <t>Bayern Mun 5-1 Dortmund</t>
+    <t>Bayern Munich 5-1 Dortmund</t>
   </si>
   <si>
     <t>B M'gladbach 2-0 VfL Wolfsburg</t>
@@ -3416,25 +3416,25 @@
     <t>Hertha BSC 3-0 Hamburger SV</t>
   </si>
   <si>
-    <t>TSG 1899 Hoffenheim 2-2 VfB Stuttgart</t>
+    <t>Hoffenheim 2-2 VfB Stuttgart</t>
   </si>
   <si>
     <t>Friday 2nd October 2015</t>
   </si>
   <si>
-    <t>SV Darmstadt 98 2-3 1. FSV Mainz 05</t>
+    <t>Darmstadt 98 2-3 Mainz 05</t>
   </si>
   <si>
     <t>Eintracht Frankfurt 1-1 Hertha BSC</t>
   </si>
   <si>
-    <t>Dortmund 2-2 SV Darmstadt 98</t>
-  </si>
-  <si>
-    <t>1. FSV Mainz 05 0-3 Bayern Mun</t>
-  </si>
-  <si>
-    <t>FC Augsburg 1-3 TSG 1899 Hoffenheim</t>
+    <t>Dortmund 2-2 Darmstadt 98</t>
+  </si>
+  <si>
+    <t>Mainz 05 0-3 Bayern Munich</t>
+  </si>
+  <si>
+    <t>FC Augsburg 1-3 Hoffenheim</t>
   </si>
   <si>
     <t>SV Werder Bremen 0-3 Bayer Levkn</t>
@@ -3458,7 +3458,7 @@
     <t>Wednesday 23rd September 2015</t>
   </si>
   <si>
-    <t>Bayer Levkn 1-0 1. FSV Mainz 05</t>
+    <t>Bayer Levkn 1-0 Mainz 05</t>
   </si>
   <si>
     <t>B M'gladbach 4-2 FC Augsburg</t>
@@ -3470,13 +3470,13 @@
     <t>Hannover 96 1-3 VfB Stuttgart</t>
   </si>
   <si>
-    <t>TSG 1899 Hoffenheim 1-1 Dortmund</t>
+    <t>Hoffenheim 1-1 Dortmund</t>
   </si>
   <si>
     <t>Tuesday 22nd September 2015</t>
   </si>
   <si>
-    <t>Bayern Mun 5-1 VfL Wolfsburg</t>
+    <t>Bayern Munich 5-1 VfL Wolfsburg</t>
   </si>
   <si>
     <t>FC Ingolstadt 04 0-1 Hamburger SV</t>
@@ -3485,7 +3485,7 @@
     <t>Hertha BSC 2-0 1. FC Köln</t>
   </si>
   <si>
-    <t>SV Darmstadt 98 2-1 SV Werder Bremen</t>
+    <t>Darmstadt 98 2-1 SV Werder Bremen</t>
   </si>
   <si>
     <t>VfB Stuttgart 0-1 Schalke</t>
@@ -3503,7 +3503,7 @@
     <t>Hamburger SV 0-0 Eintracht Frankfurt</t>
   </si>
   <si>
-    <t>SV Darmstadt 98 0-3 Bayern Mun</t>
+    <t>Darmstadt 98 0-3 Bayern Munich</t>
   </si>
   <si>
     <t>SV Werder Bremen 0-1 FC Ingolstadt 04</t>
@@ -3515,19 +3515,19 @@
     <t>Friday 18th September 2015</t>
   </si>
   <si>
-    <t>1. FSV Mainz 05 3-1 TSG 1899 Hoffenheim</t>
-  </si>
-  <si>
-    <t>TSG 1899 Hoffenheim 1-3 SV Werder Bremen</t>
-  </si>
-  <si>
-    <t>Schalke 2-1 1. FSV Mainz 05</t>
-  </si>
-  <si>
-    <t>Bayer Levkn 0-1 SV Darmstadt 98</t>
-  </si>
-  <si>
-    <t>Bayern Mun 2-1 FC Augsburg</t>
+    <t>Mainz 05 3-1 Hoffenheim</t>
+  </si>
+  <si>
+    <t>Hoffenheim 1-3 SV Werder Bremen</t>
+  </si>
+  <si>
+    <t>Schalke 2-1 Mainz 05</t>
+  </si>
+  <si>
+    <t>Bayer Levkn 0-1 Darmstadt 98</t>
+  </si>
+  <si>
+    <t>Bayern Munich 2-1 FC Augsburg</t>
   </si>
   <si>
     <t>FC Ingolstadt 04 0-0 VfL Wolfsburg</t>
@@ -3557,19 +3557,19 @@
     <t>1. FC Köln 2-1 Hamburger SV</t>
   </si>
   <si>
-    <t>1. FSV Mainz 05 3-0 Hannover 96</t>
+    <t>Mainz 05 3-0 Hannover 96</t>
   </si>
   <si>
     <t>FC Augsburg 0-1 FC Ingolstadt 04</t>
   </si>
   <si>
-    <t>SV Darmstadt 98 0-0 TSG 1899 Hoffenheim</t>
+    <t>Darmstadt 98 0-0 Hoffenheim</t>
   </si>
   <si>
     <t>VfB Stuttgart 1-4 Eintracht Frankfurt</t>
   </si>
   <si>
-    <t>Bayern Mun 3-0 Bayer Levkn</t>
+    <t>Bayern Munich 3-0 Bayer Levkn</t>
   </si>
   <si>
     <t>Friday 28th August 2015</t>
@@ -3581,7 +3581,7 @@
     <t>FC Ingolstadt 04 0-4 Dortmund</t>
   </si>
   <si>
-    <t>B M'gladbach 1-2 1. FSV Mainz 05</t>
+    <t>B M'gladbach 1-2 Mainz 05</t>
   </si>
   <si>
     <t>1. FC Köln 1-1 VfL Wolfsburg</t>
@@ -3590,13 +3590,13 @@
     <t>Eintracht Frankfurt 1-1 FC Augsburg</t>
   </si>
   <si>
-    <t>Schalke 1-1 SV Darmstadt 98</t>
+    <t>Schalke 1-1 Darmstadt 98</t>
   </si>
   <si>
     <t>Hannover 96 0-1 Bayer Levkn</t>
   </si>
   <si>
-    <t>TSG 1899 Hoffenheim 1-2 Bayern Mun</t>
+    <t>Hoffenheim 1-2 Bayern Munich</t>
   </si>
   <si>
     <t>Hamburger SV 3-2 VfB Stuttgart</t>
@@ -3614,16 +3614,16 @@
     <t>VfB Stuttgart 1-3 1. FC Köln</t>
   </si>
   <si>
-    <t>1. FSV Mainz 05 0-1 FC Ingolstadt 04</t>
-  </si>
-  <si>
-    <t>Bayer Levkn 2-1 TSG 1899 Hoffenheim</t>
+    <t>Mainz 05 0-1 FC Ingolstadt 04</t>
+  </si>
+  <si>
+    <t>Bayer Levkn 2-1 Hoffenheim</t>
   </si>
   <si>
     <t>FC Augsburg 0-1 Hertha BSC</t>
   </si>
   <si>
-    <t>SV Darmstadt 98 2-2 Hannover 96</t>
+    <t>Darmstadt 98 2-2 Hannover 96</t>
   </si>
   <si>
     <t>SV Werder Bremen 0-3 Schalke</t>
@@ -3632,7 +3632,7 @@
     <t>Dortmund 4-0 B M'gladbach</t>
   </si>
   <si>
-    <t>Bayern Mun 5-0 Hamburger SV</t>
+    <t>Bayern Munich 5-0 Hamburger SV</t>
   </si>
   <si>
     <t>Friday 4th December 2015</t>
@@ -3644,13 +3644,13 @@
     <t>1. FC Köln V FC Augsburg</t>
   </si>
   <si>
-    <t>B M'gladbach V Bayern Mun</t>
-  </si>
-  <si>
-    <t>FC Ingolstadt 04 V TSG 1899 Hoffenheim</t>
-  </si>
-  <si>
-    <t>Hamburger SV V 1. FSV Mainz 05</t>
+    <t>B M'gladbach V Bayern Munich</t>
+  </si>
+  <si>
+    <t>FC Ingolstadt 04 V Hoffenheim</t>
+  </si>
+  <si>
+    <t>Hamburger SV V Mainz 05</t>
   </si>
   <si>
     <t>Hertha BSC V Bayer Levkn</t>
@@ -3662,25 +3662,25 @@
     <t>VfB Stuttgart V SV Werder Bremen</t>
   </si>
   <si>
-    <t>Eintracht Frankfurt V SV Darmstadt 98</t>
+    <t>Eintracht Frankfurt V Darmstadt 98</t>
   </si>
   <si>
     <t>Friday 11th December 2015</t>
   </si>
   <si>
-    <t>1. FSV Mainz 05 V VfB Stuttgart</t>
-  </si>
-  <si>
-    <t>Bayern Mun V FC Ingolstadt 04</t>
-  </si>
-  <si>
-    <t>SV Darmstadt 98 V Hertha BSC</t>
+    <t>Mainz 05 V VfB Stuttgart</t>
+  </si>
+  <si>
+    <t>Bayern Munich V FC Ingolstadt 04</t>
+  </si>
+  <si>
+    <t>Darmstadt 98 V Hertha BSC</t>
   </si>
   <si>
     <t>SV Werder Bremen V 1. FC Köln</t>
   </si>
   <si>
-    <t>TSG 1899 Hoffenheim V Hannover 96</t>
+    <t>Hoffenheim V Hannover 96</t>
   </si>
   <si>
     <t>VfL Wolfsburg V Hamburger SV</t>
@@ -3698,7 +3698,7 @@
     <t>Friday 18th December 2015</t>
   </si>
   <si>
-    <t>Schalke V TSG 1899 Hoffenheim</t>
+    <t>Schalke V Hoffenheim</t>
   </si>
   <si>
     <t>1. FC Köln V Dortmund</t>
@@ -3713,37 +3713,37 @@
     <t>Hamburger SV V FC Augsburg</t>
   </si>
   <si>
-    <t>Hannover 96 V Bayern Mun</t>
+    <t>Hannover 96 V Bayern Munich</t>
   </si>
   <si>
     <t>VfB Stuttgart V VfL Wolfsburg</t>
   </si>
   <si>
-    <t>Hertha BSC V 1. FSV Mainz 05</t>
-  </si>
-  <si>
-    <t>B M'gladbach V SV Darmstadt 98</t>
+    <t>Hertha BSC V Mainz 05</t>
+  </si>
+  <si>
+    <t>B M'gladbach V Darmstadt 98</t>
   </si>
   <si>
     <t>Friday 22nd January 2016</t>
   </si>
   <si>
-    <t>Hamburger SV V Bayern Mun</t>
+    <t>Hamburger SV V Bayern Munich</t>
   </si>
   <si>
     <t>1. FC Köln V VfB Stuttgart</t>
   </si>
   <si>
-    <t>FC Ingolstadt 04 V 1. FSV Mainz 05</t>
-  </si>
-  <si>
-    <t>Hannover 96 V SV Darmstadt 98</t>
+    <t>FC Ingolstadt 04 V Mainz 05</t>
+  </si>
+  <si>
+    <t>Hannover 96 V Darmstadt 98</t>
   </si>
   <si>
     <t>Hertha BSC V FC Augsburg</t>
   </si>
   <si>
-    <t>TSG 1899 Hoffenheim V Bayer Levkn</t>
+    <t>Hoffenheim V Bayer Levkn</t>
   </si>
   <si>
     <t>B M'gladbach V Dortmund</t>
@@ -3758,7 +3758,7 @@
     <t>Friday 29th January 2016</t>
   </si>
   <si>
-    <t>1. FSV Mainz 05 V B M'gladbach</t>
+    <t>Mainz 05 V B M'gladbach</t>
   </si>
   <si>
     <t>Saturday 30th January 2016</t>
@@ -3773,7 +3773,7 @@
     <t>FC Augsburg V Eintracht Frankfurt</t>
   </si>
   <si>
-    <t>SV Darmstadt 98 V Schalke</t>
+    <t>Darmstadt 98 V Schalke</t>
   </si>
   <si>
     <t>SV Werder Bremen V Hertha BSC</t>
@@ -3788,7 +3788,7 @@
     <t>VfL Wolfsburg V 1. FC Köln</t>
   </si>
   <si>
-    <t>Bayern Mun V TSG 1899 Hoffenheim</t>
+    <t>Bayern Munich V Hoffenheim</t>
   </si>
   <si>
     <t>Friday 5th February 2016</t>
@@ -3806,13 +3806,13 @@
     <t>Schalke V VfL Wolfsburg</t>
   </si>
   <si>
-    <t>Hannover 96 V 1. FSV Mainz 05</t>
+    <t>Hannover 96 V Mainz 05</t>
   </si>
   <si>
     <t>Hertha BSC V Dortmund</t>
   </si>
   <si>
-    <t>Bayer Levkn V Bayern Mun</t>
+    <t>Bayer Levkn V Bayern Munich</t>
   </si>
   <si>
     <t>Sunday 7th February 2016</t>
@@ -3821,28 +3821,28 @@
     <t>Hamburger SV V 1. FC Köln</t>
   </si>
   <si>
-    <t>TSG 1899 Hoffenheim V SV Darmstadt 98</t>
+    <t>Hoffenheim V Darmstadt 98</t>
   </si>
   <si>
     <t>1. FC Köln V Eintracht Frankfurt</t>
   </si>
   <si>
-    <t>1. FSV Mainz 05 V Schalke</t>
+    <t>Mainz 05 V Schalke</t>
   </si>
   <si>
     <t>Dortmund V Hannover 96</t>
   </si>
   <si>
-    <t>FC Augsburg V Bayern Mun</t>
+    <t>FC Augsburg V Bayern Munich</t>
   </si>
   <si>
     <t>Hamburger SV V B M'gladbach</t>
   </si>
   <si>
-    <t>SV Darmstadt 98 V Bayer Levkn</t>
-  </si>
-  <si>
-    <t>SV Werder Bremen V TSG 1899 Hoffenheim</t>
+    <t>Darmstadt 98 V Bayer Levkn</t>
+  </si>
+  <si>
+    <t>SV Werder Bremen V Hoffenheim</t>
   </si>
   <si>
     <t>VfB Stuttgart V Hertha BSC</t>
@@ -3863,7 +3863,7 @@
     <t>Eintracht Frankfurt V Hamburger SV</t>
   </si>
   <si>
-    <t>Bayern Mun V SV Darmstadt 98</t>
+    <t>Bayern Munich V Darmstadt 98</t>
   </si>
   <si>
     <t>FC Ingolstadt 04 V SV Werder Bremen</t>
@@ -3878,16 +3878,16 @@
     <t>Hertha BSC V VfL Wolfsburg</t>
   </si>
   <si>
-    <t>TSG 1899 Hoffenheim V 1. FSV Mainz 05</t>
+    <t>Hoffenheim V Mainz 05</t>
   </si>
   <si>
     <t>1. FC Köln V Hertha BSC</t>
   </si>
   <si>
-    <t>1. FSV Mainz 05 V Bayer Levkn</t>
-  </si>
-  <si>
-    <t>Dortmund V TSG 1899 Hoffenheim</t>
+    <t>Mainz 05 V Bayer Levkn</t>
+  </si>
+  <si>
+    <t>Dortmund V Hoffenheim</t>
   </si>
   <si>
     <t>Eintracht Frankfurt V Schalke</t>
@@ -3899,13 +3899,13 @@
     <t>Hamburger SV V FC Ingolstadt 04</t>
   </si>
   <si>
-    <t>SV Werder Bremen V SV Darmstadt 98</t>
+    <t>SV Werder Bremen V Darmstadt 98</t>
   </si>
   <si>
     <t>VfB Stuttgart V Hannover 96</t>
   </si>
   <si>
-    <t>VfL Wolfsburg V Bayern Mun</t>
+    <t>VfL Wolfsburg V Bayern Munich</t>
   </si>
   <si>
     <t>Bayer Levkn V SV Werder Bremen</t>
@@ -3914,7 +3914,7 @@
     <t>B M'gladbach V VfB Stuttgart</t>
   </si>
   <si>
-    <t>Bayern Mun V 1. FSV Mainz 05</t>
+    <t>Bayern Munich V Mainz 05</t>
   </si>
   <si>
     <t>FC Ingolstadt 04 V 1. FC Köln</t>
@@ -3929,19 +3929,19 @@
     <t>Hertha BSC V Eintracht Frankfurt</t>
   </si>
   <si>
-    <t>SV Darmstadt 98 V Dortmund</t>
-  </si>
-  <si>
-    <t>TSG 1899 Hoffenheim V FC Augsburg</t>
+    <t>Darmstadt 98 V Dortmund</t>
+  </si>
+  <si>
+    <t>Hoffenheim V FC Augsburg</t>
   </si>
   <si>
     <t>1. FC Köln V Schalke</t>
   </si>
   <si>
-    <t>1. FSV Mainz 05 V SV Darmstadt 98</t>
-  </si>
-  <si>
-    <t>Dortmund V Bayern Mun</t>
+    <t>Mainz 05 V Darmstadt 98</t>
+  </si>
+  <si>
+    <t>Dortmund V Bayern Munich</t>
   </si>
   <si>
     <t>Eintracht Frankfurt V FC Ingolstadt 04</t>
@@ -3956,7 +3956,7 @@
     <t>SV Werder Bremen V Hannover 96</t>
   </si>
   <si>
-    <t>VfB Stuttgart V TSG 1899 Hoffenheim</t>
+    <t>VfB Stuttgart V Hoffenheim</t>
   </si>
   <si>
     <t>VfL Wolfsburg V B M'gladbach</t>
@@ -3965,13 +3965,13 @@
     <t>Bayer Levkn V Hamburger SV</t>
   </si>
   <si>
-    <t>Dortmund V 1. FSV Mainz 05</t>
+    <t>Dortmund V Mainz 05</t>
   </si>
   <si>
     <t>B M'gladbach V Eintracht Frankfurt</t>
   </si>
   <si>
-    <t>Bayern Mun V SV Werder Bremen</t>
+    <t>Bayern Munich V SV Werder Bremen</t>
   </si>
   <si>
     <t>FC Ingolstadt 04 V VfB Stuttgart</t>
@@ -3983,13 +3983,13 @@
     <t>Hertha BSC V Schalke</t>
   </si>
   <si>
-    <t>SV Darmstadt 98 V FC Augsburg</t>
-  </si>
-  <si>
-    <t>TSG 1899 Hoffenheim V VfL Wolfsburg</t>
-  </si>
-  <si>
-    <t>1. FC Köln V Bayern Mun</t>
+    <t>Darmstadt 98 V FC Augsburg</t>
+  </si>
+  <si>
+    <t>Hoffenheim V VfL Wolfsburg</t>
+  </si>
+  <si>
+    <t>1. FC Köln V Bayern Munich</t>
   </si>
   <si>
     <t>Eintracht Frankfurt V Hannover 96</t>
@@ -4001,22 +4001,22 @@
     <t>Schalke V B M'gladbach</t>
   </si>
   <si>
-    <t>Hamburger SV V TSG 1899 Hoffenheim</t>
+    <t>Hamburger SV V Hoffenheim</t>
   </si>
   <si>
     <t>Hertha BSC V FC Ingolstadt 04</t>
   </si>
   <si>
-    <t>SV Werder Bremen V 1. FSV Mainz 05</t>
+    <t>SV Werder Bremen V Mainz 05</t>
   </si>
   <si>
     <t>VfB Stuttgart V Bayer Levkn</t>
   </si>
   <si>
-    <t>VfL Wolfsburg V SV Darmstadt 98</t>
-  </si>
-  <si>
-    <t>1. FSV Mainz 05 V FC Augsburg</t>
+    <t>VfL Wolfsburg V Darmstadt 98</t>
+  </si>
+  <si>
+    <t>Mainz 05 V FC Augsburg</t>
   </si>
   <si>
     <t>Bayer Levkn V VfL Wolfsburg</t>
@@ -4028,7 +4028,7 @@
     <t>B M'gladbach V Hertha BSC</t>
   </si>
   <si>
-    <t>Bayern Mun V Eintracht Frankfurt</t>
+    <t>Bayern Munich V Eintracht Frankfurt</t>
   </si>
   <si>
     <t>FC Ingolstadt 04 V Schalke</t>
@@ -4037,16 +4037,16 @@
     <t>Hannover 96 V Hamburger SV</t>
   </si>
   <si>
-    <t>SV Darmstadt 98 V VfB Stuttgart</t>
-  </si>
-  <si>
-    <t>TSG 1899 Hoffenheim V 1. FC Köln</t>
+    <t>Darmstadt 98 V VfB Stuttgart</t>
+  </si>
+  <si>
+    <t>Hoffenheim V 1. FC Köln</t>
   </si>
   <si>
     <t>1. FC Köln V Bayer Levkn</t>
   </si>
   <si>
-    <t>Eintracht Frankfurt V TSG 1899 Hoffenheim</t>
+    <t>Eintracht Frankfurt V Hoffenheim</t>
   </si>
   <si>
     <t>FC Ingolstadt 04 V B M'gladbach</t>
@@ -4055,7 +4055,7 @@
     <t>Schalke V Dortmund</t>
   </si>
   <si>
-    <t>Hamburger SV V SV Darmstadt 98</t>
+    <t>Hamburger SV V Darmstadt 98</t>
   </si>
   <si>
     <t>Hertha BSC V Hannover 96</t>
@@ -4064,13 +4064,13 @@
     <t>SV Werder Bremen V FC Augsburg</t>
   </si>
   <si>
-    <t>VfB Stuttgart V Bayern Mun</t>
-  </si>
-  <si>
-    <t>VfL Wolfsburg V 1. FSV Mainz 05</t>
-  </si>
-  <si>
-    <t>1. FSV Mainz 05 V 1. FC Köln</t>
+    <t>VfB Stuttgart V Bayern Munich</t>
+  </si>
+  <si>
+    <t>VfL Wolfsburg V Mainz 05</t>
+  </si>
+  <si>
+    <t>Mainz 05 V 1. FC Köln</t>
   </si>
   <si>
     <t>Bayer Levkn V Eintracht Frankfurt</t>
@@ -4082,28 +4082,28 @@
     <t>FC Augsburg V VfB Stuttgart</t>
   </si>
   <si>
-    <t>Bayern Mun V Schalke</t>
+    <t>Bayern Munich V Schalke</t>
   </si>
   <si>
     <t>Hannover 96 V B M'gladbach</t>
   </si>
   <si>
-    <t>SV Darmstadt 98 V FC Ingolstadt 04</t>
+    <t>Darmstadt 98 V FC Ingolstadt 04</t>
   </si>
   <si>
     <t>SV Werder Bremen V VfL Wolfsburg</t>
   </si>
   <si>
-    <t>TSG 1899 Hoffenheim V Hertha BSC</t>
-  </si>
-  <si>
-    <t>1. FC Köln V SV Darmstadt 98</t>
-  </si>
-  <si>
-    <t>B M'gladbach V TSG 1899 Hoffenheim</t>
-  </si>
-  <si>
-    <t>Eintracht Frankfurt V 1. FSV Mainz 05</t>
+    <t>Hoffenheim V Hertha BSC</t>
+  </si>
+  <si>
+    <t>1. FC Köln V Darmstadt 98</t>
+  </si>
+  <si>
+    <t>B M'gladbach V Hoffenheim</t>
+  </si>
+  <si>
+    <t>Eintracht Frankfurt V Mainz 05</t>
   </si>
   <si>
     <t>FC Ingolstadt 04 V Hannover 96</t>
@@ -4115,7 +4115,7 @@
     <t>Hamburger SV V SV Werder Bremen</t>
   </si>
   <si>
-    <t>Hertha BSC V Bayern Mun</t>
+    <t>Hertha BSC V Bayern Munich</t>
   </si>
   <si>
     <t>VfB Stuttgart V Dortmund</t>
@@ -4124,7 +4124,7 @@
     <t>VfL Wolfsburg V FC Augsburg</t>
   </si>
   <si>
-    <t>1. FSV Mainz 05 V Hamburger SV</t>
+    <t>Mainz 05 V Hamburger SV</t>
   </si>
   <si>
     <t>Bayer Levkn V Hertha BSC</t>
@@ -4136,19 +4136,19 @@
     <t>FC Augsburg V 1. FC Köln</t>
   </si>
   <si>
-    <t>Bayern Mun V B M'gladbach</t>
+    <t>Bayern Munich V B M'gladbach</t>
   </si>
   <si>
     <t>Hannover 96 V Schalke</t>
   </si>
   <si>
-    <t>SV Darmstadt 98 V Eintracht Frankfurt</t>
+    <t>Darmstadt 98 V Eintracht Frankfurt</t>
   </si>
   <si>
     <t>SV Werder Bremen V VfB Stuttgart</t>
   </si>
   <si>
-    <t>TSG 1899 Hoffenheim V FC Ingolstadt 04</t>
+    <t>Hoffenheim V FC Ingolstadt 04</t>
   </si>
   <si>
     <t>1. FC Köln V SV Werder Bremen</t>
@@ -4160,7 +4160,7 @@
     <t>Eintracht Frankfurt V Dortmund</t>
   </si>
   <si>
-    <t>FC Ingolstadt 04 V Bayern Mun</t>
+    <t>FC Ingolstadt 04 V Bayern Munich</t>
   </si>
   <si>
     <t>Schalke V FC Augsburg</t>
@@ -4169,19 +4169,19 @@
     <t>Hamburger SV V VfL Wolfsburg</t>
   </si>
   <si>
-    <t>Hannover 96 V TSG 1899 Hoffenheim</t>
-  </si>
-  <si>
-    <t>Hertha BSC V SV Darmstadt 98</t>
-  </si>
-  <si>
-    <t>VfB Stuttgart V 1. FSV Mainz 05</t>
+    <t>Hannover 96 V Hoffenheim</t>
+  </si>
+  <si>
+    <t>Hertha BSC V Darmstadt 98</t>
+  </si>
+  <si>
+    <t>VfB Stuttgart V Mainz 05</t>
   </si>
   <si>
     <t>Saturday 14th May 2016</t>
   </si>
   <si>
-    <t>1. FSV Mainz 05 V Hertha BSC</t>
+    <t>Mainz 05 V Hertha BSC</t>
   </si>
   <si>
     <t>Bayer Levkn V FC Ingolstadt 04</t>
@@ -4193,16 +4193,16 @@
     <t>FC Augsburg V Hamburger SV</t>
   </si>
   <si>
-    <t>Bayern Mun V Hannover 96</t>
-  </si>
-  <si>
-    <t>SV Darmstadt 98 V B M'gladbach</t>
+    <t>Bayern Munich V Hannover 96</t>
+  </si>
+  <si>
+    <t>Darmstadt 98 V B M'gladbach</t>
   </si>
   <si>
     <t>SV Werder Bremen V Eintracht Frankfurt</t>
   </si>
   <si>
-    <t>TSG 1899 Hoffenheim V Schalke</t>
+    <t>Hoffenheim V Schalke</t>
   </si>
   <si>
     <t>VfL Wolfsburg V VfB Stuttgart</t>
@@ -6587,7 +6587,7 @@
     <t>Angers 2-0 Lille</t>
   </si>
   <si>
-    <t>GFC Ajaccio 1-1 Lorient</t>
+    <t>Ajaccio 1-1 Lorient</t>
   </si>
   <si>
     <t>Nantes 0-0 Bastia</t>
@@ -6602,7 +6602,7 @@
     <t>Lyon 2-4 Montpellier</t>
   </si>
   <si>
-    <t>Bastia 1-2 GFC Ajaccio</t>
+    <t>Bastia 1-2 Ajaccio</t>
   </si>
   <si>
     <t>Caen 0-0 Angers</t>
@@ -6656,7 +6656,7 @@
     <t>Montpellier 2-1 Nantes</t>
   </si>
   <si>
-    <t>Reims 1-2 GFC Ajaccio</t>
+    <t>Reims 1-2 Ajaccio</t>
   </si>
   <si>
     <t>Angers 0-2 Rennes</t>
@@ -6683,7 +6683,7 @@
     <t>Bastia 1-0 Caen</t>
   </si>
   <si>
-    <t>GFC Ajaccio 2-0 Bordeaux</t>
+    <t>Ajaccio 2-0 Bordeaux</t>
   </si>
   <si>
     <t>Guingamp 2-2 Lorient</t>
@@ -6716,7 +6716,7 @@
     <t>Angers 0-0 Guingamp</t>
   </si>
   <si>
-    <t>GFC Ajaccio 3-1 Nice</t>
+    <t>Ajaccio 3-1 Nice</t>
   </si>
   <si>
     <t>Montpellier 2-0 Bastia</t>
@@ -6749,7 +6749,7 @@
     <t>Reims 0-1 Caen</t>
   </si>
   <si>
-    <t>St Etienne 2-0 GFC Ajaccio</t>
+    <t>St Etienne 2-0 Ajaccio</t>
   </si>
   <si>
     <t>Toulouse 1-2 Angers</t>
@@ -6776,7 +6776,7 @@
     <t>Angers 1-0 Bastia</t>
   </si>
   <si>
-    <t>GFC Ajaccio 2-2 Toulouse</t>
+    <t>Ajaccio 2-2 Toulouse</t>
   </si>
   <si>
     <t>Troyes 0-1 Guingamp</t>
@@ -6812,7 +6812,7 @@
     <t>Bordeaux 3-1 Lyon</t>
   </si>
   <si>
-    <t>Caen 2-0 GFC Ajaccio</t>
+    <t>Caen 2-0 Ajaccio</t>
   </si>
   <si>
     <t>Rennes 1-1 Troyes</t>
@@ -6824,7 +6824,7 @@
     <t>Montpellier 2-3 Monaco</t>
   </si>
   <si>
-    <t>GFC Ajaccio 1-1 Rennes</t>
+    <t>Ajaccio 1-1 Rennes</t>
   </si>
   <si>
     <t>Lorient 2-0 Caen</t>
@@ -6872,13 +6872,13 @@
     <t>Caen 2-1 Montpellier</t>
   </si>
   <si>
-    <t>Guingamp 2-1 GFC Ajaccio</t>
+    <t>Guingamp 2-1 Ajaccio</t>
   </si>
   <si>
     <t>Rennes 1-1 Lille</t>
   </si>
   <si>
-    <t>GFC Ajaccio 0-1 Monaco</t>
+    <t>Ajaccio 0-1 Monaco</t>
   </si>
   <si>
     <t>Nantes 0-2 Rennes</t>
@@ -6923,7 +6923,7 @@
     <t>Angers 1-1 Nice</t>
   </si>
   <si>
-    <t>Lille 1-0 GFC Ajaccio</t>
+    <t>Lille 1-0 Ajaccio</t>
   </si>
   <si>
     <t>Reims 4-1 Lorient</t>
@@ -6953,7 +6953,7 @@
     <t>Bastia 3-0 Guingamp</t>
   </si>
   <si>
-    <t>GFC Ajaccio 0-2 Angers</t>
+    <t>Ajaccio 0-2 Angers</t>
   </si>
   <si>
     <t>Nantes 1-0 Reims</t>
@@ -6974,7 +6974,7 @@
     <t>Lorient 1-1 Bastia</t>
   </si>
   <si>
-    <t>Paris St G 2-0 GFC Ajaccio</t>
+    <t>Paris St G 2-0 Ajaccio</t>
   </si>
   <si>
     <t>St Etienne 1-1 Bordeaux</t>
@@ -7022,7 +7022,7 @@
     <t>Nice 1-2 Monaco</t>
   </si>
   <si>
-    <t>Troyes 0-0 GFC Ajaccio</t>
+    <t>Troyes 0-0 Ajaccio</t>
   </si>
   <si>
     <t>Friday 7th August 2015</t>
@@ -7043,7 +7043,7 @@
     <t>Monaco V Caen</t>
   </si>
   <si>
-    <t>Montpellier V GFC Ajaccio</t>
+    <t>Montpellier V Ajaccio</t>
   </si>
   <si>
     <t>Troyes V Toulouse</t>
@@ -7070,7 +7070,7 @@
     <t>Caen V Lille</t>
   </si>
   <si>
-    <t>GFC Ajaccio V Nantes</t>
+    <t>Ajaccio V Nantes</t>
   </si>
   <si>
     <t>Reims V Troyes</t>
@@ -7112,7 +7112,7 @@
     <t>Angers V Bordeaux</t>
   </si>
   <si>
-    <t>Marseille V GFC Ajaccio</t>
+    <t>Marseille V Ajaccio</t>
   </si>
   <si>
     <t>Paris St G V Lyon</t>
@@ -7142,7 +7142,7 @@
     <t>St Etienne V Angers</t>
   </si>
   <si>
-    <t>GFC Ajaccio V Lyon</t>
+    <t>Ajaccio V Lyon</t>
   </si>
   <si>
     <t>Bordeaux V Marseille</t>
@@ -7163,7 +7163,7 @@
     <t>Marseille V Guingamp</t>
   </si>
   <si>
-    <t>Monaco V GFC Ajaccio</t>
+    <t>Monaco V Ajaccio</t>
   </si>
   <si>
     <t>Montpellier V Bordeaux</t>
@@ -7190,7 +7190,7 @@
     <t>Caen V Marseille</t>
   </si>
   <si>
-    <t>GFC Ajaccio V Reims</t>
+    <t>Ajaccio V Reims</t>
   </si>
   <si>
     <t>Guingamp V Nantes</t>
@@ -7238,7 +7238,7 @@
     <t>Reims V St Etienne</t>
   </si>
   <si>
-    <t>Rennes V GFC Ajaccio</t>
+    <t>Rennes V Ajaccio</t>
   </si>
   <si>
     <t>Angers V Monaco</t>
@@ -7253,7 +7253,7 @@
     <t>Caen V Nice</t>
   </si>
   <si>
-    <t>GFC Ajaccio V Montpellier</t>
+    <t>Ajaccio V Montpellier</t>
   </si>
   <si>
     <t>Lorient V Reims</t>
@@ -7286,7 +7286,7 @@
     <t>Montpellier V Marseille</t>
   </si>
   <si>
-    <t>Nantes V GFC Ajaccio</t>
+    <t>Nantes V Ajaccio</t>
   </si>
   <si>
     <t>Nice V Toulouse</t>
@@ -7313,7 +7313,7 @@
     <t>Caen V Reims</t>
   </si>
   <si>
-    <t>GFC Ajaccio V Guingamp</t>
+    <t>Ajaccio V Guingamp</t>
   </si>
   <si>
     <t>Lille V Rennes</t>
@@ -7331,7 +7331,7 @@
     <t>Toulouse V Nantes</t>
   </si>
   <si>
-    <t>GFC Ajaccio V Troyes</t>
+    <t>Ajaccio V Troyes</t>
   </si>
   <si>
     <t>Guingamp V Bordeaux</t>
@@ -7388,10 +7388,10 @@
     <t>Paris St G V Reims</t>
   </si>
   <si>
-    <t>Toulouse V GFC Ajaccio</t>
-  </si>
-  <si>
-    <t>GFC Ajaccio V Marseille</t>
+    <t>Toulouse V Ajaccio</t>
+  </si>
+  <si>
+    <t>Ajaccio V Marseille</t>
   </si>
   <si>
     <t>Guingamp V Angers</t>
@@ -7427,7 +7427,7 @@
     <t>Bastia V Lorient</t>
   </si>
   <si>
-    <t>Bordeaux V GFC Ajaccio</t>
+    <t>Bordeaux V Ajaccio</t>
   </si>
   <si>
     <t>Caen V Monaco</t>
@@ -7454,7 +7454,7 @@
     <t>Bastia V Lille</t>
   </si>
   <si>
-    <t>GFC Ajaccio V Caen</t>
+    <t>Ajaccio V Caen</t>
   </si>
   <si>
     <t>Guingamp V St Etienne</t>
@@ -7499,7 +7499,7 @@
     <t>Marseille V Rennes</t>
   </si>
   <si>
-    <t>Nice V GFC Ajaccio</t>
+    <t>Nice V Ajaccio</t>
   </si>
   <si>
     <t>Paris St G V Monaco</t>
@@ -7514,7 +7514,7 @@
     <t>Bastia V Marseille</t>
   </si>
   <si>
-    <t>GFC Ajaccio V St Etienne</t>
+    <t>Ajaccio V St Etienne</t>
   </si>
   <si>
     <t>Guingamp V Montpellier</t>
@@ -7541,7 +7541,7 @@
     <t>Troyes V Angers</t>
   </si>
   <si>
-    <t>Angers V GFC Ajaccio</t>
+    <t>Ajaccio V Nice</t>
   </si>
   <si>
     <t>Caen V Lorient</t>
@@ -7577,7 +7577,7 @@
     <t>Bordeaux V Angers</t>
   </si>
   <si>
-    <t>GFC Ajaccio V Lille</t>
+    <t>Ajaccio V Lille</t>
   </si>
   <si>
     <t>Lorient V Toulouse</t>
@@ -7604,7 +7604,7 @@
     <t>Bordeaux V Paris St G</t>
   </si>
   <si>
-    <t>GFC Ajaccio V Bastia</t>
+    <t>Ajaccio V Bastia</t>
   </si>
   <si>
     <t>Guingamp V Caen</t>
@@ -7640,7 +7640,7 @@
     <t>Lorient V Lille</t>
   </si>
   <si>
-    <t>Lyon V GFC Ajaccio</t>
+    <t>Lyon V Ajaccio</t>
   </si>
   <si>
     <t>Monaco V Guingamp</t>
@@ -7667,7 +7667,7 @@
     <t>Bordeaux V Lorient</t>
   </si>
   <si>
-    <t>GFC Ajaccio V Paris St G</t>
+    <t>Ajaccio V Paris St G</t>
   </si>
   <si>
     <t>Lille V Guingamp</t>
@@ -7700,7 +7700,7 @@
     <t>Guingamp V Nice</t>
   </si>
   <si>
-    <t>Lorient V GFC Ajaccio</t>
+    <t>Lorient V Ajaccio</t>
   </si>
   <si>
     <t>Monaco V Montpellier</t>
@@ -11716,26 +11716,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A27:K27"/>
     <mergeCell ref="A23:K23"/>
+    <mergeCell ref="A24:K24"/>
     <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A26:K26"/>
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="A30:K30"/>
+    <mergeCell ref="A29:K29"/>
     <mergeCell ref="A34:K34"/>
     <mergeCell ref="A33:K33"/>
+    <mergeCell ref="A28:K28"/>
+    <mergeCell ref="A31:K31"/>
+    <mergeCell ref="A32:K32"/>
     <mergeCell ref="A36:K36"/>
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="A31:K31"/>
-    <mergeCell ref="A30:K30"/>
     <mergeCell ref="A38:K38"/>
     <mergeCell ref="A41:K41"/>
     <mergeCell ref="A40:K40"/>
     <mergeCell ref="A39:K39"/>
     <mergeCell ref="A37:K37"/>
-    <mergeCell ref="A28:K28"/>
-    <mergeCell ref="A27:K27"/>
-    <mergeCell ref="A26:K26"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="A29:K29"/>
-    <mergeCell ref="A32:K32"/>
+    <mergeCell ref="A35:K35"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -12358,42 +12358,42 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A138:K138"/>
-    <mergeCell ref="A136:K136"/>
-    <mergeCell ref="A144:K144"/>
-    <mergeCell ref="A142:K142"/>
-    <mergeCell ref="A130:K130"/>
-    <mergeCell ref="A140:K140"/>
-    <mergeCell ref="A146:K146"/>
-    <mergeCell ref="A148:K148"/>
-    <mergeCell ref="A150:K150"/>
-    <mergeCell ref="A132:K132"/>
-    <mergeCell ref="A134:K134"/>
+    <mergeCell ref="A16:K16"/>
+    <mergeCell ref="A18:K18"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="A8:K8"/>
     <mergeCell ref="A10:K10"/>
     <mergeCell ref="A12:K12"/>
-    <mergeCell ref="A16:K16"/>
     <mergeCell ref="A14:K14"/>
+    <mergeCell ref="A124:K124"/>
+    <mergeCell ref="A126:K126"/>
+    <mergeCell ref="A134:K134"/>
+    <mergeCell ref="A138:K138"/>
+    <mergeCell ref="A136:K136"/>
+    <mergeCell ref="A144:K144"/>
+    <mergeCell ref="A142:K142"/>
+    <mergeCell ref="A132:K132"/>
+    <mergeCell ref="A140:K140"/>
+    <mergeCell ref="A130:K130"/>
+    <mergeCell ref="A128:K128"/>
+    <mergeCell ref="A148:K148"/>
+    <mergeCell ref="A150:K150"/>
     <mergeCell ref="A118:K118"/>
     <mergeCell ref="A120:K120"/>
     <mergeCell ref="A122:K122"/>
-    <mergeCell ref="A124:K124"/>
-    <mergeCell ref="A126:K126"/>
-    <mergeCell ref="A128:K128"/>
+    <mergeCell ref="A116:K116"/>
+    <mergeCell ref="A146:K146"/>
     <mergeCell ref="A28:K28"/>
+    <mergeCell ref="A26:K26"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="A36:K36"/>
     <mergeCell ref="A30:K30"/>
     <mergeCell ref="A32:K32"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="A18:K18"/>
     <mergeCell ref="A20:K20"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A26:K26"/>
-    <mergeCell ref="A116:K116"/>
-    <mergeCell ref="A36:K36"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -13080,26 +13080,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A20:K20"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A14:K14"/>
     <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A2:K2"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="A8:K8"/>
     <mergeCell ref="A10:K10"/>
+    <mergeCell ref="A12:K12"/>
     <mergeCell ref="A28:K28"/>
     <mergeCell ref="A30:K30"/>
-    <mergeCell ref="A32:K32"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A26:K26"/>
     <mergeCell ref="A34:K34"/>
     <mergeCell ref="A36:K36"/>
     <mergeCell ref="A38:K38"/>
     <mergeCell ref="A40:K40"/>
     <mergeCell ref="A16:K16"/>
-    <mergeCell ref="A14:K14"/>
     <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A20:K20"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A26:K26"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="A32:K32"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -13786,26 +13786,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A20:K20"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A14:K14"/>
     <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A2:K2"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="A8:K8"/>
     <mergeCell ref="A10:K10"/>
+    <mergeCell ref="A12:K12"/>
     <mergeCell ref="A28:K28"/>
     <mergeCell ref="A30:K30"/>
-    <mergeCell ref="A32:K32"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A26:K26"/>
     <mergeCell ref="A34:K34"/>
     <mergeCell ref="A36:K36"/>
     <mergeCell ref="A38:K38"/>
     <mergeCell ref="A40:K40"/>
     <mergeCell ref="A16:K16"/>
-    <mergeCell ref="A14:K14"/>
     <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A20:K20"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A26:K26"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="A32:K32"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -14492,26 +14492,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A20:K20"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A14:K14"/>
     <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A2:K2"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="A8:K8"/>
     <mergeCell ref="A10:K10"/>
+    <mergeCell ref="A12:K12"/>
     <mergeCell ref="A28:K28"/>
     <mergeCell ref="A30:K30"/>
-    <mergeCell ref="A32:K32"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A26:K26"/>
     <mergeCell ref="A34:K34"/>
     <mergeCell ref="A36:K36"/>
     <mergeCell ref="A38:K38"/>
     <mergeCell ref="A40:K40"/>
     <mergeCell ref="A16:K16"/>
-    <mergeCell ref="A14:K14"/>
     <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A20:K20"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A26:K26"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="A32:K32"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -14802,7 +14802,7 @@
         <v>185</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>65</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13">
@@ -14811,19 +14811,19 @@
         <v>70</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>71</v>
@@ -14835,19 +14835,19 @@
         <v>77</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>78</v>
@@ -14859,19 +14859,19 @@
         <v>83</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>83</v>
@@ -14883,19 +14883,19 @@
         <v>88</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>89</v>
@@ -14907,19 +14907,19 @@
         <v>94</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I17" s="9" t="s">
         <v>94</v>
@@ -14931,19 +14931,19 @@
         <v>101</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I18" s="9" t="s">
         <v>102</v>
@@ -14955,19 +14955,19 @@
         <v>107</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I19" s="9" t="s">
         <v>108</v>
@@ -14979,19 +14979,19 @@
         <v>113</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="I20" s="9" t="s">
         <v>113</v>
@@ -15003,19 +15003,19 @@
         <v>119</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I21" s="9" t="s">
         <v>120</v>
@@ -15027,19 +15027,19 @@
         <v>124</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="I22" s="9" t="s">
         <v>125</v>
@@ -15057,19 +15057,19 @@
         <v>9</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H25" s="9"/>
       <c r="I25" s="10" t="s">
@@ -15082,19 +15082,19 @@
         <v>15</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H26" s="9"/>
       <c r="I26" s="11" t="s">
@@ -15103,23 +15103,23 @@
     </row>
     <row r="27">
       <c r="A27" s="9"/>
-      <c r="B27" s="9" t="s">
-        <v>22</v>
+      <c r="B27" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="H27" s="9"/>
       <c r="I27" s="10" t="s">
@@ -15132,19 +15132,19 @@
         <v>28</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H28" s="9"/>
       <c r="I28" s="10" t="s">
@@ -15157,19 +15157,19 @@
         <v>34</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="H29" s="9"/>
       <c r="I29" s="11" t="s">
@@ -15182,19 +15182,19 @@
         <v>41</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="10" t="s">
@@ -15207,22 +15207,22 @@
         <v>47</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>48</v>
+        <v>269</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="32">
@@ -15231,19 +15231,19 @@
         <v>53</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="I32" s="10" t="s">
         <v>53</v>
@@ -15255,19 +15255,19 @@
         <v>59</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H33" s="9"/>
       <c r="I33" s="10" t="s">
@@ -15280,19 +15280,19 @@
         <v>66</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H34" s="9"/>
       <c r="I34" s="10" t="s">
@@ -15305,19 +15305,19 @@
         <v>72</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="H35" s="9"/>
       <c r="I35" s="10" t="s">
@@ -15330,19 +15330,19 @@
         <v>79</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="H36" s="9"/>
       <c r="I36" s="9" t="s">
@@ -15355,19 +15355,19 @@
         <v>84</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H37" s="9"/>
       <c r="I37" s="12" t="s">
@@ -15380,19 +15380,19 @@
         <v>90</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="I38" s="13" t="s">
         <v>90</v>
@@ -15404,19 +15404,19 @@
         <v>95</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="H39" s="9"/>
       <c r="I39" s="11" t="s">
@@ -15429,19 +15429,19 @@
         <v>103</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="I40" s="10" t="s">
         <v>103</v>
@@ -15453,19 +15453,19 @@
         <v>109</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="11" t="s">
@@ -15478,19 +15478,19 @@
         <v>114</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H42" s="9"/>
       <c r="I42" s="12" t="s">
@@ -15508,22 +15508,22 @@
         <v>10</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="I45" s="8" t="s">
         <v>11</v>
@@ -15535,22 +15535,22 @@
         <v>17</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H46" s="8" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="I46" s="8" t="s">
         <v>18</v>
@@ -15562,22 +15562,22 @@
         <v>24</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="I47" s="8" t="s">
         <v>24</v>
@@ -15589,22 +15589,22 @@
         <v>30</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="I48" s="8" t="s">
         <v>30</v>
@@ -15616,22 +15616,22 @@
         <v>36</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="H49" s="8" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="I49" s="8" t="s">
         <v>36</v>
@@ -15643,22 +15643,22 @@
         <v>42</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="I50" s="8" t="s">
         <v>42</v>
@@ -15670,22 +15670,22 @@
         <v>49</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="I51" s="8" t="s">
         <v>49</v>
@@ -15697,22 +15697,22 @@
         <v>54</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="I52" s="8" t="s">
         <v>54</v>
@@ -15724,22 +15724,22 @@
         <v>60</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="I53" s="8" t="s">
         <v>60</v>
@@ -15751,22 +15751,22 @@
         <v>67</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="I54" s="8" t="s">
         <v>67</v>
@@ -15778,22 +15778,22 @@
         <v>74</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="I55" s="8" t="s">
         <v>74</v>
@@ -15805,20 +15805,20 @@
         <v>80</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F56" s="19"/>
       <c r="G56" s="9" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="H56" s="8" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="I56" s="8" t="s">
         <v>80</v>
@@ -15830,22 +15830,22 @@
         <v>85</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="H57" s="8" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="I57" s="8" t="s">
         <v>85</v>
@@ -15857,20 +15857,20 @@
         <v>91</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F58" s="19"/>
       <c r="G58" s="9" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="I58" s="8" t="s">
         <v>91</v>
@@ -15882,22 +15882,22 @@
         <v>97</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="I59" s="8" t="s">
         <v>97</v>
@@ -15909,22 +15909,22 @@
         <v>104</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="I60" s="8" t="s">
         <v>104</v>
@@ -15936,20 +15936,20 @@
         <v>110</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="F61" s="19"/>
       <c r="G61" s="9" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="H61" s="8" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="I61" s="8" t="s">
         <v>110</v>
@@ -15961,22 +15961,22 @@
         <v>115</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="H62" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I62" s="8" t="s">
         <v>115</v>
@@ -15988,22 +15988,22 @@
         <v>121</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="H63" s="8" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="I63" s="8" t="s">
         <v>121</v>
@@ -16015,22 +16015,22 @@
         <v>126</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="H64" s="8" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="I64" s="8" t="s">
         <v>126</v>
@@ -16047,22 +16047,22 @@
         <v>12</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="G67" s="9" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="H67" s="9" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="I67" s="9" t="s">
         <v>12</v>
@@ -16074,19 +16074,19 @@
         <v>19</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="H68" s="9" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="I68" s="9" t="s">
         <v>19</v>
@@ -16098,22 +16098,22 @@
         <v>25</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="H69" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="I69" s="9" t="s">
         <v>25</v>
@@ -16125,22 +16125,22 @@
         <v>31</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="H70" s="9" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="I70" s="9" t="s">
         <v>31</v>
@@ -16152,22 +16152,22 @@
         <v>37</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="H71" s="9" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="I71" s="9" t="s">
         <v>37</v>
@@ -16179,22 +16179,22 @@
         <v>43</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="H72" s="9" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="I72" s="9" t="s">
         <v>43</v>
@@ -16206,22 +16206,22 @@
         <v>50</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="H73" s="9" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="I73" s="9" t="s">
         <v>50</v>
@@ -16233,22 +16233,22 @@
         <v>55</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="H74" s="9" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="I74" s="9" t="s">
         <v>55</v>
@@ -16260,22 +16260,22 @@
         <v>61</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="H75" s="9" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="I75" s="9" t="s">
         <v>62</v>
@@ -16287,22 +16287,22 @@
         <v>68</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="H76" s="9" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="I76" s="9" t="s">
         <v>68</v>
@@ -16314,22 +16314,22 @@
         <v>75</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G77" s="9" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="H77" s="9" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="I77" s="9" t="s">
         <v>75</v>
@@ -16341,19 +16341,19 @@
         <v>81</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="H78" s="9" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="I78" s="9" t="s">
         <v>81</v>
@@ -16365,22 +16365,22 @@
         <v>86</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="G79" s="9" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="H79" s="9" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="I79" s="9" t="s">
         <v>86</v>
@@ -16392,22 +16392,22 @@
         <v>92</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="G80" s="9" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="H80" s="9" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="I80" s="9" t="s">
         <v>92</v>
@@ -16419,19 +16419,19 @@
         <v>98</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="G81" s="9" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="H81" s="9" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="I81" s="9" t="s">
         <v>98</v>
@@ -16443,19 +16443,19 @@
         <v>105</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G82" s="9" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="H82" s="9" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="I82" s="9" t="s">
         <v>105</v>
@@ -16467,22 +16467,22 @@
         <v>111</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="G83" s="9" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="H83" s="9" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="I83" s="9" t="s">
         <v>111</v>
@@ -16494,22 +16494,22 @@
         <v>116</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="G84" s="9" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="H84" s="9" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="I84" s="9" t="s">
         <v>116</v>
@@ -16521,22 +16521,22 @@
         <v>122</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="G85" s="9" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="H85" s="9" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="I85" s="9" t="s">
         <v>122</v>
@@ -16548,22 +16548,22 @@
         <v>127</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="F86" s="9" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="G86" s="9" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="H86" s="9" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="I86" s="9" t="s">
         <v>127</v>
@@ -16571,7 +16571,7 @@
     </row>
     <row r="88">
       <c r="A88" s="20" t="s">
-        <v>518</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89">
@@ -16586,7 +16586,7 @@
         <v>520</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F89" s="8" t="s">
         <v>521</v>
@@ -16610,7 +16610,7 @@
         <v>524</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F90" s="8" t="s">
         <v>525</v>
@@ -16634,7 +16634,7 @@
         <v>528</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F91" s="8" t="s">
         <v>529</v>
@@ -16659,7 +16659,7 @@
         <v>532</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F92" s="8" t="s">
         <v>533</v>
@@ -16684,7 +16684,7 @@
         <v>536</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="F93" s="8" t="s">
         <v>537</v>
@@ -16734,7 +16734,7 @@
         <v>545</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F95" s="8" t="s">
         <v>546</v>
@@ -16759,7 +16759,7 @@
         <v>549</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F96" s="8" t="s">
         <v>550</v>
@@ -16784,7 +16784,7 @@
         <v>553</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F97" s="8" t="s">
         <v>554</v>
@@ -16809,7 +16809,7 @@
         <v>557</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F98" s="8" t="s">
         <v>558</v>
@@ -16834,7 +16834,7 @@
         <v>561</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F99" s="8" t="s">
         <v>562</v>
@@ -16859,7 +16859,7 @@
         <v>565</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F100" s="8" t="s">
         <v>566</v>
@@ -16934,7 +16934,7 @@
         <v>579</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F103" s="8" t="s">
         <v>580</v>
@@ -16983,7 +16983,7 @@
         <v>588</v>
       </c>
       <c r="E105" s="8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F105" s="8" t="s">
         <v>589</v>
@@ -17008,7 +17008,7 @@
         <v>592</v>
       </c>
       <c r="E106" s="8" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F106" s="8" t="s">
         <v>593</v>
@@ -17032,7 +17032,7 @@
         <v>596</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F107" s="8" t="s">
         <v>597</v>
@@ -17057,7 +17057,7 @@
         <v>600</v>
       </c>
       <c r="E108" s="8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F108" s="8" t="s">
         <v>601</v>
@@ -21507,38 +21507,30 @@
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="B787:C787"/>
-    <mergeCell ref="B793:C793"/>
+    <mergeCell ref="B799:C799"/>
+    <mergeCell ref="B819:C819"/>
+    <mergeCell ref="B829:C829"/>
+    <mergeCell ref="B847:C847"/>
+    <mergeCell ref="B853:C853"/>
+    <mergeCell ref="B859:C859"/>
+    <mergeCell ref="B889:C889"/>
+    <mergeCell ref="B879:C879"/>
     <mergeCell ref="B727:C727"/>
+    <mergeCell ref="B709:C709"/>
+    <mergeCell ref="B699:C699"/>
+    <mergeCell ref="B679:C679"/>
+    <mergeCell ref="B673:C673"/>
+    <mergeCell ref="B667:C667"/>
+    <mergeCell ref="B651:C651"/>
+    <mergeCell ref="B639:C639"/>
+    <mergeCell ref="B592:C592"/>
     <mergeCell ref="B733:C733"/>
     <mergeCell ref="B741:C741"/>
     <mergeCell ref="B759:C759"/>
     <mergeCell ref="B771:C771"/>
-    <mergeCell ref="B709:C709"/>
-    <mergeCell ref="B699:C699"/>
-    <mergeCell ref="B176:C176"/>
-    <mergeCell ref="B184:C184"/>
-    <mergeCell ref="B196:C196"/>
-    <mergeCell ref="B212:C212"/>
-    <mergeCell ref="B230:C230"/>
-    <mergeCell ref="B238:C238"/>
-    <mergeCell ref="B244:C244"/>
-    <mergeCell ref="B264:C264"/>
-    <mergeCell ref="B272:C272"/>
-    <mergeCell ref="B294:C294"/>
-    <mergeCell ref="B300:C300"/>
-    <mergeCell ref="B324:C324"/>
-    <mergeCell ref="B348:C348"/>
-    <mergeCell ref="B372:C372"/>
-    <mergeCell ref="B973:C973"/>
-    <mergeCell ref="B983:C983"/>
-    <mergeCell ref="B889:C889"/>
-    <mergeCell ref="B907:C907"/>
-    <mergeCell ref="B913:C913"/>
-    <mergeCell ref="B921:C921"/>
-    <mergeCell ref="B939:C939"/>
-    <mergeCell ref="B947:C947"/>
-    <mergeCell ref="B967:C967"/>
+    <mergeCell ref="B787:C787"/>
+    <mergeCell ref="B793:C793"/>
+    <mergeCell ref="B616:C616"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B30:C30"/>
@@ -21553,36 +21545,44 @@
     <mergeCell ref="B144:C144"/>
     <mergeCell ref="B150:C150"/>
     <mergeCell ref="B156:C156"/>
-    <mergeCell ref="B799:C799"/>
-    <mergeCell ref="B819:C819"/>
-    <mergeCell ref="B829:C829"/>
-    <mergeCell ref="B847:C847"/>
-    <mergeCell ref="B853:C853"/>
-    <mergeCell ref="B859:C859"/>
-    <mergeCell ref="B879:C879"/>
-    <mergeCell ref="B639:C639"/>
-    <mergeCell ref="B616:C616"/>
-    <mergeCell ref="B679:C679"/>
-    <mergeCell ref="B673:C673"/>
-    <mergeCell ref="B667:C667"/>
-    <mergeCell ref="B651:C651"/>
-    <mergeCell ref="B544:C544"/>
-    <mergeCell ref="B568:C568"/>
-    <mergeCell ref="B592:C592"/>
-    <mergeCell ref="B394:C394"/>
-    <mergeCell ref="B400:C400"/>
+    <mergeCell ref="B973:C973"/>
+    <mergeCell ref="B983:C983"/>
+    <mergeCell ref="B999:C999"/>
+    <mergeCell ref="B1005:C1005"/>
+    <mergeCell ref="B967:C967"/>
+    <mergeCell ref="B1041:C1041"/>
+    <mergeCell ref="B1051:C1051"/>
+    <mergeCell ref="B1029:C1029"/>
+    <mergeCell ref="B1035:C1035"/>
+    <mergeCell ref="B1013:C1013"/>
     <mergeCell ref="B424:C424"/>
     <mergeCell ref="B448:C448"/>
     <mergeCell ref="B472:C472"/>
     <mergeCell ref="B496:C496"/>
+    <mergeCell ref="B544:C544"/>
+    <mergeCell ref="B568:C568"/>
+    <mergeCell ref="B394:C394"/>
+    <mergeCell ref="B400:C400"/>
     <mergeCell ref="B520:C520"/>
-    <mergeCell ref="B1041:C1041"/>
-    <mergeCell ref="B1051:C1051"/>
-    <mergeCell ref="B1029:C1029"/>
-    <mergeCell ref="B1035:C1035"/>
-    <mergeCell ref="B999:C999"/>
-    <mergeCell ref="B1005:C1005"/>
-    <mergeCell ref="B1013:C1013"/>
+    <mergeCell ref="B372:C372"/>
+    <mergeCell ref="B907:C907"/>
+    <mergeCell ref="B913:C913"/>
+    <mergeCell ref="B921:C921"/>
+    <mergeCell ref="B939:C939"/>
+    <mergeCell ref="B947:C947"/>
+    <mergeCell ref="B264:C264"/>
+    <mergeCell ref="B272:C272"/>
+    <mergeCell ref="B294:C294"/>
+    <mergeCell ref="B300:C300"/>
+    <mergeCell ref="B324:C324"/>
+    <mergeCell ref="B348:C348"/>
+    <mergeCell ref="B176:C176"/>
+    <mergeCell ref="B184:C184"/>
+    <mergeCell ref="B196:C196"/>
+    <mergeCell ref="B212:C212"/>
+    <mergeCell ref="B230:C230"/>
+    <mergeCell ref="B238:C238"/>
+    <mergeCell ref="B244:C244"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -25301,54 +25301,30 @@
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="B798:C798"/>
-    <mergeCell ref="B820:C820"/>
-    <mergeCell ref="B666:C666"/>
-    <mergeCell ref="B842:C842"/>
-    <mergeCell ref="B864:C864"/>
-    <mergeCell ref="B886:C886"/>
-    <mergeCell ref="B776:C776"/>
-    <mergeCell ref="B688:C688"/>
-    <mergeCell ref="B754:C754"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="B178:C178"/>
+    <mergeCell ref="B154:C154"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="B330:C330"/>
+    <mergeCell ref="B338:C338"/>
+    <mergeCell ref="B270:C270"/>
+    <mergeCell ref="B258:C258"/>
     <mergeCell ref="B280:C280"/>
     <mergeCell ref="B294:C294"/>
     <mergeCell ref="B300:C300"/>
     <mergeCell ref="B308:C308"/>
     <mergeCell ref="B324:C324"/>
-    <mergeCell ref="B330:C330"/>
-    <mergeCell ref="B354:C354"/>
-    <mergeCell ref="B338:C338"/>
-    <mergeCell ref="B360:C360"/>
-    <mergeCell ref="B368:C368"/>
-    <mergeCell ref="B384:C384"/>
-    <mergeCell ref="B390:C390"/>
-    <mergeCell ref="B398:C398"/>
-    <mergeCell ref="B414:C414"/>
-    <mergeCell ref="B270:C270"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="B154:C154"/>
-    <mergeCell ref="B162:C162"/>
-    <mergeCell ref="B178:C178"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="B420:C420"/>
-    <mergeCell ref="B426:C426"/>
-    <mergeCell ref="B442:C442"/>
-    <mergeCell ref="B450:C450"/>
-    <mergeCell ref="B456:C456"/>
-    <mergeCell ref="B472:C472"/>
-    <mergeCell ref="B480:C480"/>
-    <mergeCell ref="B486:C486"/>
     <mergeCell ref="B502:C502"/>
     <mergeCell ref="B510:C510"/>
     <mergeCell ref="B516:C516"/>
@@ -25362,18 +25338,42 @@
     <mergeCell ref="B600:C600"/>
     <mergeCell ref="B622:C622"/>
     <mergeCell ref="B644:C644"/>
-    <mergeCell ref="B710:C710"/>
-    <mergeCell ref="B732:C732"/>
-    <mergeCell ref="B184:C184"/>
-    <mergeCell ref="B194:C194"/>
+    <mergeCell ref="B666:C666"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B360:C360"/>
+    <mergeCell ref="B368:C368"/>
+    <mergeCell ref="B384:C384"/>
+    <mergeCell ref="B390:C390"/>
+    <mergeCell ref="B398:C398"/>
+    <mergeCell ref="B354:C354"/>
+    <mergeCell ref="B414:C414"/>
+    <mergeCell ref="B420:C420"/>
+    <mergeCell ref="B426:C426"/>
+    <mergeCell ref="B442:C442"/>
+    <mergeCell ref="B450:C450"/>
+    <mergeCell ref="B456:C456"/>
+    <mergeCell ref="B472:C472"/>
+    <mergeCell ref="B480:C480"/>
+    <mergeCell ref="B486:C486"/>
     <mergeCell ref="B208:C208"/>
     <mergeCell ref="B214:C214"/>
     <mergeCell ref="B222:C222"/>
     <mergeCell ref="B238:C238"/>
+    <mergeCell ref="B194:C194"/>
+    <mergeCell ref="B184:C184"/>
     <mergeCell ref="B244:C244"/>
-    <mergeCell ref="B258:C258"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B776:C776"/>
+    <mergeCell ref="B732:C732"/>
+    <mergeCell ref="B754:C754"/>
+    <mergeCell ref="B798:C798"/>
+    <mergeCell ref="B842:C842"/>
+    <mergeCell ref="B864:C864"/>
+    <mergeCell ref="B886:C886"/>
+    <mergeCell ref="B820:C820"/>
+    <mergeCell ref="B688:C688"/>
+    <mergeCell ref="B710:C710"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -29737,6 +29737,17 @@
   <mergeCells count="76">
     <mergeCell ref="B150:C150"/>
     <mergeCell ref="B162:C162"/>
+    <mergeCell ref="B168:C168"/>
+    <mergeCell ref="B174:C174"/>
+    <mergeCell ref="B186:C186"/>
+    <mergeCell ref="B200:C200"/>
+    <mergeCell ref="B212:C212"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B54:C54"/>
     <mergeCell ref="B80:C80"/>
     <mergeCell ref="B94:C94"/>
     <mergeCell ref="B100:C100"/>
@@ -29744,73 +29755,62 @@
     <mergeCell ref="B126:C126"/>
     <mergeCell ref="B132:C132"/>
     <mergeCell ref="B138:C138"/>
-    <mergeCell ref="B226:C226"/>
-    <mergeCell ref="B232:C232"/>
-    <mergeCell ref="B168:C168"/>
-    <mergeCell ref="B174:C174"/>
-    <mergeCell ref="B186:C186"/>
-    <mergeCell ref="B200:C200"/>
-    <mergeCell ref="B212:C212"/>
-    <mergeCell ref="B244:C244"/>
-    <mergeCell ref="B258:C258"/>
-    <mergeCell ref="B322:C322"/>
-    <mergeCell ref="B328:C328"/>
-    <mergeCell ref="B264:C264"/>
-    <mergeCell ref="B270:C270"/>
-    <mergeCell ref="B286:C286"/>
-    <mergeCell ref="B334:C334"/>
-    <mergeCell ref="B346:C346"/>
-    <mergeCell ref="B296:C296"/>
-    <mergeCell ref="B310:C310"/>
-    <mergeCell ref="B364:C364"/>
-    <mergeCell ref="B378:C378"/>
-    <mergeCell ref="B390:C390"/>
-    <mergeCell ref="B396:C396"/>
-    <mergeCell ref="B402:C402"/>
-    <mergeCell ref="B414:C414"/>
-    <mergeCell ref="B446:C446"/>
-    <mergeCell ref="B458:C458"/>
-    <mergeCell ref="B464:C464"/>
-    <mergeCell ref="B470:C470"/>
-    <mergeCell ref="B484:C484"/>
-    <mergeCell ref="B496:C496"/>
-    <mergeCell ref="B358:C358"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B726:C726"/>
+    <mergeCell ref="B732:C732"/>
+    <mergeCell ref="B780:C780"/>
     <mergeCell ref="B804:C804"/>
     <mergeCell ref="B828:C828"/>
     <mergeCell ref="B852:C852"/>
-    <mergeCell ref="B876:C876"/>
-    <mergeCell ref="B780:C780"/>
     <mergeCell ref="B756:C756"/>
+    <mergeCell ref="B900:C900"/>
     <mergeCell ref="B924:C924"/>
     <mergeCell ref="B948:C948"/>
     <mergeCell ref="B972:C972"/>
     <mergeCell ref="B996:C996"/>
     <mergeCell ref="B1020:C1020"/>
     <mergeCell ref="B1044:C1044"/>
-    <mergeCell ref="B900:C900"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B876:C876"/>
+    <mergeCell ref="B414:C414"/>
     <mergeCell ref="B432:C432"/>
+    <mergeCell ref="B446:C446"/>
+    <mergeCell ref="B458:C458"/>
+    <mergeCell ref="B464:C464"/>
+    <mergeCell ref="B470:C470"/>
     <mergeCell ref="B426:C426"/>
+    <mergeCell ref="B346:C346"/>
+    <mergeCell ref="B358:C358"/>
+    <mergeCell ref="B364:C364"/>
+    <mergeCell ref="B378:C378"/>
+    <mergeCell ref="B390:C390"/>
+    <mergeCell ref="B396:C396"/>
+    <mergeCell ref="B402:C402"/>
+    <mergeCell ref="B258:C258"/>
+    <mergeCell ref="B264:C264"/>
+    <mergeCell ref="B226:C226"/>
+    <mergeCell ref="B232:C232"/>
+    <mergeCell ref="B244:C244"/>
+    <mergeCell ref="B334:C334"/>
+    <mergeCell ref="B270:C270"/>
+    <mergeCell ref="B286:C286"/>
+    <mergeCell ref="B296:C296"/>
+    <mergeCell ref="B310:C310"/>
+    <mergeCell ref="B322:C322"/>
+    <mergeCell ref="B328:C328"/>
+    <mergeCell ref="B576:C576"/>
+    <mergeCell ref="B582:C582"/>
     <mergeCell ref="B606:C606"/>
     <mergeCell ref="B630:C630"/>
     <mergeCell ref="B654:C654"/>
     <mergeCell ref="B678:C678"/>
     <mergeCell ref="B702:C702"/>
-    <mergeCell ref="B726:C726"/>
-    <mergeCell ref="B732:C732"/>
+    <mergeCell ref="B484:C484"/>
+    <mergeCell ref="B496:C496"/>
     <mergeCell ref="B508:C508"/>
     <mergeCell ref="B522:C522"/>
     <mergeCell ref="B544:C544"/>
     <mergeCell ref="B550:C550"/>
     <mergeCell ref="B560:C560"/>
-    <mergeCell ref="B576:C576"/>
-    <mergeCell ref="B582:C582"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -34586,70 +34586,70 @@
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="B632:C632"/>
+    <mergeCell ref="B656:C656"/>
+    <mergeCell ref="B728:C728"/>
+    <mergeCell ref="B704:C704"/>
     <mergeCell ref="B1032:C1032"/>
     <mergeCell ref="B992:C992"/>
     <mergeCell ref="B944:C944"/>
     <mergeCell ref="B968:C968"/>
+    <mergeCell ref="B920:C920"/>
     <mergeCell ref="B776:C776"/>
     <mergeCell ref="B800:C800"/>
-    <mergeCell ref="B824:C824"/>
     <mergeCell ref="B848:C848"/>
     <mergeCell ref="B872:C872"/>
     <mergeCell ref="B896:C896"/>
-    <mergeCell ref="B920:C920"/>
-    <mergeCell ref="B338:C338"/>
+    <mergeCell ref="B536:C536"/>
+    <mergeCell ref="B560:C560"/>
+    <mergeCell ref="B584:C584"/>
+    <mergeCell ref="B608:C608"/>
+    <mergeCell ref="B680:C680"/>
+    <mergeCell ref="B752:C752"/>
+    <mergeCell ref="B824:C824"/>
     <mergeCell ref="B384:C384"/>
     <mergeCell ref="B392:C392"/>
-    <mergeCell ref="B412:C412"/>
-    <mergeCell ref="B420:C420"/>
-    <mergeCell ref="B426:C426"/>
-    <mergeCell ref="B464:C464"/>
-    <mergeCell ref="B452:C452"/>
-    <mergeCell ref="B536:C536"/>
-    <mergeCell ref="B560:C560"/>
-    <mergeCell ref="B184:C184"/>
-    <mergeCell ref="B174:C174"/>
-    <mergeCell ref="B232:C232"/>
-    <mergeCell ref="B240:C240"/>
-    <mergeCell ref="B248:C248"/>
-    <mergeCell ref="B264:C264"/>
-    <mergeCell ref="B272:C272"/>
-    <mergeCell ref="B278:C278"/>
-    <mergeCell ref="B298:C298"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B212:C212"/>
-    <mergeCell ref="B204:C204"/>
-    <mergeCell ref="B156:C156"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B704:C704"/>
-    <mergeCell ref="B608:C608"/>
-    <mergeCell ref="B632:C632"/>
-    <mergeCell ref="B656:C656"/>
-    <mergeCell ref="B680:C680"/>
-    <mergeCell ref="B434:C434"/>
-    <mergeCell ref="B478:C478"/>
-    <mergeCell ref="B484:C484"/>
-    <mergeCell ref="B490:C490"/>
-    <mergeCell ref="B364:C364"/>
-    <mergeCell ref="B354:C354"/>
-    <mergeCell ref="B304:C304"/>
-    <mergeCell ref="B324:C324"/>
-    <mergeCell ref="B332:C332"/>
-    <mergeCell ref="B728:C728"/>
-    <mergeCell ref="B752:C752"/>
-    <mergeCell ref="B584:C584"/>
-    <mergeCell ref="B512:C512"/>
     <mergeCell ref="B92:C92"/>
     <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B100:C100"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B174:C174"/>
+    <mergeCell ref="B184:C184"/>
+    <mergeCell ref="B204:C204"/>
+    <mergeCell ref="B278:C278"/>
     <mergeCell ref="B130:C130"/>
-    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B156:C156"/>
+    <mergeCell ref="B212:C212"/>
+    <mergeCell ref="B248:C248"/>
+    <mergeCell ref="B464:C464"/>
+    <mergeCell ref="B478:C478"/>
+    <mergeCell ref="B484:C484"/>
+    <mergeCell ref="B490:C490"/>
+    <mergeCell ref="B354:C354"/>
+    <mergeCell ref="B324:C324"/>
+    <mergeCell ref="B332:C332"/>
+    <mergeCell ref="B338:C338"/>
+    <mergeCell ref="B512:C512"/>
+    <mergeCell ref="B364:C364"/>
+    <mergeCell ref="B452:C452"/>
+    <mergeCell ref="B412:C412"/>
+    <mergeCell ref="B420:C420"/>
+    <mergeCell ref="B426:C426"/>
+    <mergeCell ref="B434:C434"/>
+    <mergeCell ref="B240:C240"/>
+    <mergeCell ref="B232:C232"/>
+    <mergeCell ref="B272:C272"/>
+    <mergeCell ref="B264:C264"/>
+    <mergeCell ref="B298:C298"/>
+    <mergeCell ref="B304:C304"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -38462,7 +38462,7 @@
       </c>
     </row>
     <row r="930">
-      <c r="A930" s="26" t="s">
+      <c r="A930" s="22" t="s">
         <v>819</v>
       </c>
     </row>
@@ -39045,25 +39045,56 @@
     </row>
   </sheetData>
   <mergeCells count="78">
+    <mergeCell ref="B310:C310"/>
+    <mergeCell ref="B322:C322"/>
+    <mergeCell ref="B496:C496"/>
+    <mergeCell ref="B448:C448"/>
+    <mergeCell ref="B464:C464"/>
+    <mergeCell ref="B470:C470"/>
+    <mergeCell ref="B480:C480"/>
+    <mergeCell ref="B400:C400"/>
+    <mergeCell ref="B406:C406"/>
+    <mergeCell ref="B416:C416"/>
+    <mergeCell ref="B432:C432"/>
+    <mergeCell ref="B438:C438"/>
+    <mergeCell ref="B342:C342"/>
+    <mergeCell ref="B352:C352"/>
+    <mergeCell ref="B302:C302"/>
+    <mergeCell ref="B384:C384"/>
+    <mergeCell ref="B368:C368"/>
+    <mergeCell ref="B374:C374"/>
+    <mergeCell ref="B336:C336"/>
+    <mergeCell ref="B242:C242"/>
     <mergeCell ref="B286:C286"/>
-    <mergeCell ref="B302:C302"/>
-    <mergeCell ref="B224:C224"/>
-    <mergeCell ref="B236:C236"/>
-    <mergeCell ref="B242:C242"/>
     <mergeCell ref="B248:C248"/>
     <mergeCell ref="B260:C260"/>
     <mergeCell ref="B274:C274"/>
     <mergeCell ref="B280:C280"/>
-    <mergeCell ref="B368:C368"/>
-    <mergeCell ref="B374:C374"/>
-    <mergeCell ref="B310:C310"/>
-    <mergeCell ref="B322:C322"/>
-    <mergeCell ref="B336:C336"/>
-    <mergeCell ref="B342:C342"/>
-    <mergeCell ref="B352:C352"/>
-    <mergeCell ref="B384:C384"/>
-    <mergeCell ref="B400:C400"/>
+    <mergeCell ref="B160:C160"/>
+    <mergeCell ref="B172:C172"/>
+    <mergeCell ref="B180:C180"/>
+    <mergeCell ref="B190:C190"/>
+    <mergeCell ref="B206:C206"/>
+    <mergeCell ref="B212:C212"/>
+    <mergeCell ref="B236:C236"/>
+    <mergeCell ref="B224:C224"/>
+    <mergeCell ref="B908:C908"/>
+    <mergeCell ref="B932:C932"/>
+    <mergeCell ref="B956:C956"/>
+    <mergeCell ref="B980:C980"/>
+    <mergeCell ref="B1004:C1004"/>
+    <mergeCell ref="B1028:C1028"/>
+    <mergeCell ref="B1052:C1052"/>
+    <mergeCell ref="B884:C884"/>
+    <mergeCell ref="B740:C740"/>
+    <mergeCell ref="B764:C764"/>
+    <mergeCell ref="B788:C788"/>
+    <mergeCell ref="B812:C812"/>
+    <mergeCell ref="B836:C836"/>
+    <mergeCell ref="B860:C860"/>
     <mergeCell ref="B588:C588"/>
+    <mergeCell ref="B576:C576"/>
+    <mergeCell ref="B716:C716"/>
     <mergeCell ref="B594:C594"/>
     <mergeCell ref="B610:C610"/>
     <mergeCell ref="B620:C620"/>
@@ -39071,58 +39102,27 @@
     <mergeCell ref="B668:C668"/>
     <mergeCell ref="B692:C692"/>
     <mergeCell ref="B518:C518"/>
+    <mergeCell ref="B502:C502"/>
     <mergeCell ref="B524:C524"/>
     <mergeCell ref="B530:C530"/>
     <mergeCell ref="B546:C546"/>
     <mergeCell ref="B556:C556"/>
     <mergeCell ref="B562:C562"/>
-    <mergeCell ref="B576:C576"/>
-    <mergeCell ref="B884:C884"/>
-    <mergeCell ref="B908:C908"/>
-    <mergeCell ref="B932:C932"/>
-    <mergeCell ref="B956:C956"/>
-    <mergeCell ref="B980:C980"/>
-    <mergeCell ref="B1004:C1004"/>
-    <mergeCell ref="B1028:C1028"/>
-    <mergeCell ref="B1052:C1052"/>
-    <mergeCell ref="B716:C716"/>
-    <mergeCell ref="B740:C740"/>
-    <mergeCell ref="B764:C764"/>
-    <mergeCell ref="B788:C788"/>
-    <mergeCell ref="B812:C812"/>
-    <mergeCell ref="B836:C836"/>
-    <mergeCell ref="B860:C860"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="B142:C142"/>
     <mergeCell ref="B78:C78"/>
     <mergeCell ref="B88:C88"/>
     <mergeCell ref="B104:C104"/>
     <mergeCell ref="B110:C110"/>
     <mergeCell ref="B116:C116"/>
     <mergeCell ref="B126:C126"/>
-    <mergeCell ref="B142:C142"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="B160:C160"/>
-    <mergeCell ref="B172:C172"/>
-    <mergeCell ref="B180:C180"/>
-    <mergeCell ref="B190:C190"/>
-    <mergeCell ref="B206:C206"/>
-    <mergeCell ref="B212:C212"/>
-    <mergeCell ref="B406:C406"/>
-    <mergeCell ref="B416:C416"/>
-    <mergeCell ref="B432:C432"/>
-    <mergeCell ref="B438:C438"/>
-    <mergeCell ref="B448:C448"/>
-    <mergeCell ref="B480:C480"/>
-    <mergeCell ref="B496:C496"/>
-    <mergeCell ref="B464:C464"/>
-    <mergeCell ref="B470:C470"/>
-    <mergeCell ref="B502:C502"/>
+    <mergeCell ref="B72:C72"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -39136,7 +39136,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="49.43"/>
-    <col customWidth="1" min="2" max="2" width="4.0"/>
+    <col customWidth="1" min="2" max="2" width="10.86"/>
+    <col customWidth="1" min="4" max="4" width="78.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -50553,51 +50554,51 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="B733:E733"/>
-    <mergeCell ref="B736:E736"/>
     <mergeCell ref="B754:E754"/>
     <mergeCell ref="B757:E757"/>
-    <mergeCell ref="B629:D629"/>
+    <mergeCell ref="B723:E723"/>
+    <mergeCell ref="C719:E719"/>
     <mergeCell ref="B653:D653"/>
-    <mergeCell ref="C719:E719"/>
-    <mergeCell ref="B723:E723"/>
+    <mergeCell ref="B677:D677"/>
+    <mergeCell ref="B557:D557"/>
+    <mergeCell ref="B581:D581"/>
     <mergeCell ref="B726:E726"/>
+    <mergeCell ref="B736:E736"/>
+    <mergeCell ref="C739:E739"/>
+    <mergeCell ref="B733:E733"/>
     <mergeCell ref="C729:E729"/>
-    <mergeCell ref="C739:E739"/>
-    <mergeCell ref="B677:D677"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="B79:D79"/>
-    <mergeCell ref="B97:D97"/>
-    <mergeCell ref="B103:D103"/>
-    <mergeCell ref="B117:D117"/>
-    <mergeCell ref="B129:D129"/>
-    <mergeCell ref="B141:D141"/>
-    <mergeCell ref="B155:D155"/>
-    <mergeCell ref="B177:D177"/>
-    <mergeCell ref="B91:D91"/>
-    <mergeCell ref="B183:D183"/>
-    <mergeCell ref="B193:D193"/>
+    <mergeCell ref="B263:D263"/>
+    <mergeCell ref="B311:D311"/>
+    <mergeCell ref="B287:D287"/>
     <mergeCell ref="B209:D209"/>
     <mergeCell ref="B215:D215"/>
+    <mergeCell ref="B155:D155"/>
     <mergeCell ref="B239:D239"/>
-    <mergeCell ref="B263:D263"/>
-    <mergeCell ref="B287:D287"/>
+    <mergeCell ref="B629:D629"/>
     <mergeCell ref="B461:D461"/>
     <mergeCell ref="B485:D485"/>
+    <mergeCell ref="B605:D605"/>
+    <mergeCell ref="B177:D177"/>
     <mergeCell ref="B509:D509"/>
     <mergeCell ref="B533:D533"/>
-    <mergeCell ref="B557:D557"/>
-    <mergeCell ref="B581:D581"/>
-    <mergeCell ref="B605:D605"/>
-    <mergeCell ref="B311:D311"/>
     <mergeCell ref="B335:D335"/>
     <mergeCell ref="B359:D359"/>
     <mergeCell ref="B365:D365"/>
     <mergeCell ref="B389:D389"/>
     <mergeCell ref="B413:D413"/>
     <mergeCell ref="B437:D437"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B79:D79"/>
+    <mergeCell ref="B103:D103"/>
+    <mergeCell ref="B117:D117"/>
+    <mergeCell ref="B97:D97"/>
+    <mergeCell ref="B91:D91"/>
+    <mergeCell ref="B141:D141"/>
+    <mergeCell ref="B129:D129"/>
+    <mergeCell ref="B183:D183"/>
+    <mergeCell ref="B193:D193"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>